<commit_message>
feat: Simpler test and treatments descriptions and background information
</commit_message>
<xml_diff>
--- a/Analysis/tests_treatments_enhanced_analysis.xlsx
+++ b/Analysis/tests_treatments_enhanced_analysis.xlsx
@@ -670,12 +670,12 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>Arterial blood gas analysis is a blood test that measures the levels of oxygen and carbon dioxide in the blood, as well as blood pH.  It assesses the body's ability to effectively exchange gases and maintain acid-base balance.</t>
+          <t>It's a blood test that measures the levels of oxygen and carbon dioxide in your blood.</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>This test is performed to evaluate respiratory function and acid-base balance in patients with suspected or confirmed respiratory disorders, metabolic disturbances, or acid-base imbalances. It helps diagnose and monitor conditions affecting oxygenation, ventilation, and acid-base homeostasis. Information not found regarding specific conditions this test helps treat.</t>
+          <t>Doctors use this test when they want to check how well your lungs and kidneys are working, or if you have breathing problems.</t>
         </is>
       </c>
       <c r="E9" s="5" t="inlineStr">
@@ -705,12 +705,12 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Arthroscopy is a minimally invasive surgical procedure involving the insertion of a thin, fiber-optic instrument (arthroscope) into a joint to visualize and treat internal structures.  It allows for diagnosis and treatment of joint injuries and diseases.</t>
+          <t>Arthroscopy is a surgery where a doctor inserts a thin tube with a camera into a joint to see inside and repair damage.</t>
         </is>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
-          <t>Arthroscopy is used to diagnose and treat a variety of joint problems, including tears in cartilage or ligaments, bone fractures, and inflammation. It allows for direct visualization of the joint, enabling surgeons to perform minimally invasive repairs, remove loose bodies, and obtain tissue samples for biopsy.  The procedure is typically performed when less invasive methods fail to provide a clear diagnosis or effective treatment.</t>
+          <t>Doctors use arthroscopy to diagnose and treat problems in joints like knees, shoulders, and ankles.</t>
         </is>
       </c>
       <c r="E10" s="6" t="inlineStr">
@@ -735,17 +735,17 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>Análisis de sangre; Hemograma completo (for CBC specifically)</t>
+          <t>Análisis de sangre</t>
         </is>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>A blood test is a laboratory procedure that analyzes a sample of blood to assess various health parameters.  It measures different components of the blood, including red and white blood cells, hemoglobin, hematocrit, and platelets, providing insights into overall health and potential underlying conditions.  Results can indicate the presence of infection, anemia, or other blood disorders.</t>
+          <t>A blood test checks your blood to see if everything is okay.</t>
         </is>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>Blood tests, such as the complete blood count (CBC), are routinely used for general health checks, to diagnose a wide range of conditions based on abnormal cell counts (e.g., anemia, infection, leukemia), to monitor the progression of existing conditions, and to assess the effectiveness of treatments affecting blood cells (e.g., chemotherapy, radiation).  It is ordered when a patient presents with symptoms like fatigue, weakness, fever, bruising, or bleeding.</t>
+          <t>Doctors order blood tests to check your overall health or to help find out what's wrong when you're sick.</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr">
@@ -770,17 +770,17 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>Análisis de sangre; Hemograma completo</t>
+          <t>No encontrado en Mayo Clinic</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>Blood tests, specifically a complete blood count (CBC), analyze components of blood, including red and white blood cells, hemoglobin, hematocrit, and platelets.  This provides information about overall health and helps detect various medical conditions.</t>
+          <t>Not found on Mayo Clinic</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
-          <t>A CBC is a common blood test used as part of a routine medical exam, to diagnose the cause of symptoms (e.g., weakness, fatigue, fever), to monitor existing medical conditions affecting blood cell counts, and to track the effects of treatments like medications or radiation that impact blood cells.  It's performed by drawing a blood sample from a vein.</t>
+          <t>Not found on Mayo Clinic</t>
         </is>
       </c>
       <c r="E12" s="6" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="G12" s="6" t="inlineStr">
         <is>
-          <t>https://www.mayoclinic.org/tests-procedures/complete-blood-count/about/pac-20384919</t>
+          <t>Not found</t>
         </is>
       </c>
     </row>
@@ -810,12 +810,12 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>El cálculo del índice de masa corporal (IMC) es un método simple para evaluar el peso en relación con la talla.  Se utiliza para clasificar a los individuos en categorías de peso como bajo peso, peso normal, sobrepeso y obesidad.  El IMC proporciona una estimación general del nivel de grasa corporal.</t>
+          <t>It's a way to figure out if someone is a healthy weight based on their height and weight.</t>
         </is>
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>El cálculo del IMC se realiza como una herramienta de cribado para identificar el riesgo de enfermedades relacionadas con el peso.  Se utiliza ampliamente en la práctica clínica para evaluar el estado nutricional,  monitorizar cambios de peso y determinar la necesidad de intervenciones para la pérdida de peso o el manejo de la obesidad.  Ayuda a identificar a individuos con mayor riesgo de desarrollar enfermedades como la diabetes tipo 2, enfermedades cardiovasculares y ciertos tipos de cáncer.</t>
+          <t>Doctors use it to check if a person's weight might be causing health problems.</t>
         </is>
       </c>
       <c r="E13" s="5" t="inlineStr">
@@ -845,12 +845,12 @@
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Cardiac catheterization is a minimally invasive procedure used to diagnose and treat certain heart conditions.  A thin, flexible tube (catheter) is inserted into a blood vessel and guided to the heart to visualize the chambers and blood vessels, assess blood flow, and potentially perform interventions.</t>
+          <t>It's a procedure where a thin, flexible tube is inserted into a blood vessel to check the heart and blood vessels.</t>
         </is>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
-          <t>This test is used to evaluate various heart conditions, including coronary artery disease, heart valve problems, and congenital heart defects.  It helps assess blood flow, detect blockages, and measure pressures within the heart chambers.  Cardiac catheterization can also be used to perform interventions such as angioplasty or stent placement.</t>
+          <t>Doctors use this test to see if there are problems with the heart or blood vessels, such as blockages.</t>
         </is>
       </c>
       <c r="E14" s="6" t="inlineStr">
@@ -875,17 +875,17 @@
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>Ecografía carótida; Ultrasonido carotídeo</t>
+          <t>Ecografía carótida</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>A carotid ultrasound is a non-invasive imaging test that uses sound waves to visualize the carotid arteries in the neck.  It assesses the blood flow and identifies potential blockages or narrowing (stenosis) within these arteries.</t>
+          <t>It's a test that uses sound waves to create pictures of the carotid arteries in your neck.</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>This test is used to screen for and diagnose carotid artery disease, a condition where plaque buildup narrows the arteries, reducing blood flow to the brain.  It's performed when a patient presents with symptoms suggestive of stroke or transient ischemic attack (TIA), or as a preventative measure in individuals with risk factors for stroke such as high blood pressure, high cholesterol, diabetes, or a family history of stroke.  The ultrasound helps evaluate the severity of stenosis and guide treatment decisions, such as medication, surgery, or lifestyle modifications.</t>
+          <t>Doctors use this test to check for problems with blood flow in the neck arteries.</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr">
@@ -915,12 +915,12 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>A cerebral angiogram is a diagnostic imaging procedure that uses X-rays and a special contrast dye to visualize the blood vessels in the brain.  It provides detailed images of the arteries and veins to detect blockages, aneurysms, or other abnormalities.</t>
+          <t>It's a picture of the blood vessels in your brain.</t>
         </is>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
-          <t>This test is used to evaluate a variety of cerebrovascular conditions. It's performed when there is suspicion of a stroke, aneurysm, arteriovenous malformation (AVM), stenosis, or other vascular abnormalities in the brain.  The procedure helps diagnose and guide treatment for these conditions.</t>
+          <t>Doctors use it to check for problems with blood flow in the brain.</t>
         </is>
       </c>
       <c r="E16" s="6" t="inlineStr">
@@ -950,12 +950,12 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>A chest X-ray is a non-invasive imaging technique using X-radiation to produce images of the structures within the chest, including the lungs, heart, blood vessels, and bones.  It helps visualize abnormalities such as pneumonia, lung cancer, and pleural effusions.</t>
+          <t>It's a picture of your lungs and heart taken with X-rays.</t>
         </is>
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>Chest X-rays are used to diagnose a wide range of respiratory and cardiovascular conditions. They are frequently ordered when a patient presents with symptoms such as cough, shortness of breath, chest pain, or fever.  The test can detect abnormalities like infections, tumors, fluid buildup, and bone fractures.</t>
+          <t>Doctors use it to check for problems in your lungs and heart.</t>
         </is>
       </c>
       <c r="E17" s="5" t="inlineStr">
@@ -980,17 +980,17 @@
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>Prueba de colesterol;  Análisis de colesterol</t>
+          <t>Prueba de colesterol</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>A cholesterol test measures the levels of cholesterol and other fats (lipids) in the blood.  These levels are important indicators of cardiovascular health and risk for heart disease.  The test helps assess the need for lifestyle changes or medical interventions.</t>
+          <t>It's a blood test that measures the amount of cholesterol in your blood.</t>
         </is>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t>Cholesterol tests are routinely used as part of preventative care, particularly for adults, to assess cardiovascular risk.  They are also performed to monitor cholesterol levels in individuals with known heart disease or high cholesterol, to evaluate the effectiveness of cholesterol-lowering medications, and to screen for underlying conditions like hyperlipidemia. This helps diagnose and manage conditions related to elevated or low cholesterol levels.</t>
+          <t>Doctors order this test to check for heart disease risk and to monitor cholesterol levels.</t>
         </is>
       </c>
       <c r="E18" s="6" t="inlineStr">
@@ -1020,12 +1020,12 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>Cognitive and neuropsychological tests assess various cognitive functions, including memory, attention, language, and executive functions. These tests help identify cognitive impairments and determine their severity, guiding diagnosis and treatment planning.</t>
+          <t>These tests check how well your brain works by assessing memory, thinking, and problem-solving skills.</t>
         </is>
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>These tests are used to evaluate cognitive function in individuals suspected of having cognitive disorders or experiencing cognitive decline. They are performed to diagnose conditions affecting cognitive abilities, monitor disease progression, and assess treatment effectiveness.  They are helpful in a wide range of situations, including suspected dementia, traumatic brain injury, learning disabilities, and the effects of neurological diseases.</t>
+          <t>Doctors use these tests when they suspect someone might have a brain injury, dementia, or other problems affecting thinking skills.</t>
         </is>
       </c>
       <c r="E19" s="5" t="inlineStr">
@@ -1055,12 +1055,12 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>A complete blood count (CBC) is a blood test that measures various components of blood, including red blood cells, white blood cells, platelets, hemoglobin, and hematocrit.  It provides a broad overview of a person's overall health and can detect a wide range of medical conditions.</t>
+          <t>It's a blood test that checks your blood cells to see if everything is okay.</t>
         </is>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
-          <t>A CBC is a common blood test used as part of a routine medical exam, to diagnose the cause of symptoms like fatigue, fever, or bleeding, to monitor the progress of a medical condition affecting blood cell counts, and to track the effects of medical treatments (e.g., chemotherapy, radiation).  It helps assess overall health and detect conditions like anemia, infection, and leukemia.</t>
+          <t>Doctors order this test to check your overall health, diagnose illnesses, or monitor conditions affecting your blood.</t>
         </is>
       </c>
       <c r="E20" s="6" t="inlineStr">
@@ -1090,12 +1090,12 @@
       </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>It's a special X-ray that takes many pictures to create detailed images of the inside of your body.</t>
         </is>
       </c>
       <c r="D21" s="5" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use it to look for problems inside your body, like injuries, infections, or tumors.</t>
         </is>
       </c>
       <c r="E21" s="5" t="inlineStr">
@@ -1125,12 +1125,12 @@
       </c>
       <c r="C22" s="6" t="inlineStr">
         <is>
-          <t>Computerized tomography angiography (CTA) is a medical imaging technique that combines computed tomography (CT) scanning with the injection of an iodinated contrast agent to visualize blood vessels.  It provides detailed three-dimensional images of arteries and veins, allowing for the assessment of blood flow and the detection of abnormalities.</t>
+          <t>It's a special X-ray that uses a computer to make detailed pictures of blood vessels.</t>
         </is>
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
-          <t>CTA is used to diagnose a wide range of vascular conditions.  It's performed when there's suspicion of blockage, narrowing, or aneurysm in blood vessels.  The procedure helps assess the severity of vascular diseases and guide treatment planning. Information not found regarding specific conditions it helps treat.</t>
+          <t>Doctors use this test to check for problems with blood vessels, like blockages or narrowing.</t>
         </is>
       </c>
       <c r="E22" s="6" t="inlineStr">
@@ -1160,12 +1160,12 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>A CT scan (computed tomography scan) is a medical imaging procedure that uses X-rays to create detailed cross-sectional images of the body.  These images allow doctors to visualize internal organs, bones, and tissues in greater detail than traditional X-rays.</t>
+          <t>It's a type of scan that takes detailed pictures of the inside of your body.</t>
         </is>
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>CT scans are used to diagnose a wide range of conditions affecting various parts of the body. They are employed when detailed internal imaging is required to assess injuries, detect tumors, evaluate internal bleeding, or assess the extent of disease.  The specific reason for ordering a CT scan will depend on the patient's symptoms and medical history. Information not found regarding specific conditions it helps treat.</t>
+          <t>Doctors use it to look for problems inside your body, like injuries or diseases.</t>
         </is>
       </c>
       <c r="E23" s="5" t="inlineStr">
@@ -1195,12 +1195,12 @@
       </c>
       <c r="C24" s="6" t="inlineStr">
         <is>
-          <t>An echocardiogram is a non-invasive cardiac examination that uses ultrasound to visualize the heart's structure and function.  It assesses heart valve function, chamber size, and blood flow to detect abnormalities.</t>
+          <t>An echocardiogram is a test that uses sound waves to create a moving picture of the heart.</t>
         </is>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
-          <t>Echocardiograms are used to diagnose and monitor various heart conditions. They are performed to evaluate symptoms like chest pain, shortness of breath, and palpitations, as well as to assess the effectiveness of treatment for existing cardiac diseases.</t>
+          <t>Doctors use this test to check how well the heart is working and to look for problems with the heart's structure.</t>
         </is>
       </c>
       <c r="E24" s="6" t="inlineStr">
@@ -1230,12 +1230,12 @@
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>An electrocardiogram (ECG or EKG) is a simple, non-invasive test that measures the electrical activity of the heart.  It records the heart's rhythm and electrical conduction pathways, detecting abnormalities in heart rate and rhythm.</t>
+          <t>It's a test that checks your heart's rhythm and electrical activity.</t>
         </is>
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>Electrocardiograms are used to diagnose a wide range of heart conditions, including arrhythmias, coronary artery disease, and myocardial infarction. They are often performed as part of a routine physical examination, to evaluate symptoms such as chest pain or palpitations, or to monitor the effectiveness of heart medications.  The test helps assess heart function and identify potential problems before they cause significant health issues.</t>
+          <t>Doctors use this test to check for heart problems or to monitor the heart's health.</t>
         </is>
       </c>
       <c r="E25" s="5" t="inlineStr">
@@ -1260,17 +1260,17 @@
       </c>
       <c r="B26" s="6" t="inlineStr">
         <is>
-          <t>Prueba de esfuerzo con electrocardiograma</t>
+          <t>Prueba de esfuerzo</t>
         </is>
       </c>
       <c r="C26" s="6" t="inlineStr">
         <is>
-          <t>An exercise stress test is a non-invasive diagnostic test that assesses the heart's response to physical exertion. It monitors heart rate, rhythm, and blood pressure while the patient exercises on a treadmill or stationary bike to detect potential cardiovascular issues.</t>
+          <t>It's a test where you exercise while your heart is monitored to see how well it works.</t>
         </is>
       </c>
       <c r="D26" s="6" t="inlineStr">
         <is>
-          <t>This test is used to evaluate individuals with symptoms suggestive of coronary artery disease (CAD), such as chest pain (angina), shortness of breath, or dizziness during exertion. It helps determine the presence and severity of CAD by observing how well the heart performs under stress.  It can also help assess the effectiveness of treatments for heart conditions.</t>
+          <t>Doctors use this test when they want to check how your heart handles physical activity and to look for heart problems.</t>
         </is>
       </c>
       <c r="E26" s="6" t="inlineStr">
@@ -1300,12 +1300,12 @@
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>Exercise tests, also known as stress tests, assess cardiovascular function by monitoring heart rate, rhythm, and blood pressure during controlled physical exertion.  These tests help evaluate the heart's response to stress and identify potential abnormalities.</t>
+          <t>It's a test that checks how your heart works when you exercise.</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>Exercise tests are used to diagnose or manage various heart conditions, such as coronary artery disease, valvular heart disease, and arrhythmias. They are performed when there is suspicion of heart disease based on symptoms like chest pain or shortness of breath.  The test helps determine the extent of heart disease and guide treatment decisions.</t>
+          <t>Doctors use it to see if your heart is healthy enough for physical activity or to find heart problems.</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
@@ -1330,17 +1330,17 @@
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>Tomografía Computarizada Cardíaca;  TAC Cardíaca</t>
+          <t>Tomografía computarizada del corazón</t>
         </is>
       </c>
       <c r="C28" s="6" t="inlineStr">
         <is>
-          <t>A heart CT scan (also known as cardiac CT) is a non-invasive imaging technique using X-rays to create detailed cross-sectional images of the heart and its surrounding structures.  It provides information about coronary artery disease, heart structure, and other cardiovascular conditions.</t>
+          <t>It's a special x-ray that takes pictures of your heart to see how it's working.</t>
         </is>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
-          <t>A heart CT scan is used to assess coronary artery disease, detect blockages in the coronary arteries, evaluate heart valve function, and identify congenital heart defects. It's performed when there's suspicion of heart disease based on symptoms or risk factors.  The scan aids in diagnosis and treatment planning.</t>
+          <t>Doctors use it to check for problems with your heart like blockages or damage.</t>
         </is>
       </c>
       <c r="E28" s="6" t="inlineStr">
@@ -1365,17 +1365,17 @@
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>Resonancia magnética cardiaca; Imagen por resonancia magnética del corazón</t>
+          <t>Resonancia magnética cardíaca</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
         <is>
-          <t>Heart magnetic resonance imaging (MRI) is a non-invasive medical imaging technique that uses a powerful magnetic field and radio waves to produce detailed images of the heart and its surrounding structures.  It provides information about the heart's size, shape, function, and blood flow.</t>
+          <t>It's a special scan that uses magnets and radio waves to take detailed pictures of the heart.</t>
         </is>
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>A heart MRI is used to evaluate a wide range of cardiac conditions. It is performed to assess heart function after a heart attack, detect congenital heart defects, evaluate the effectiveness of treatments, and diagnose or monitor various heart diseases.  The test helps visualize heart structures, assess blood flow, and identify abnormalities not readily apparent through other methods.</t>
+          <t>Doctors use this test to check for problems with the heart's structure and how well it's working.</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr">
@@ -1405,12 +1405,12 @@
       </c>
       <c r="C30" s="6" t="inlineStr">
         <is>
-          <t>Holter monitoring is a diagnostic test that involves continuous electrocardiographic (ECG) recording over a 24-48 hour period using a portable device. This allows for detection of cardiac arrhythmias and other abnormalities that may not be apparent during a routine ECG.</t>
+          <t>It's a test that records your heart's rhythm and electrical activity over a period of time.</t>
         </is>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>Holter monitoring is used when there is suspicion of intermittent cardiac arrhythmias, palpitations, or syncope. It helps identify the frequency, duration, and characteristics of arrhythmias, aiding in diagnosis and management of heart conditions. This test is useful in evaluating patients with symptoms suggestive of cardiac issues or in monitoring the effectiveness of cardiac medications.</t>
+          <t>Doctors use this test when they suspect a problem with your heart rhythm or to find the cause of symptoms like dizziness or palpitations.</t>
         </is>
       </c>
       <c r="E30" s="6" t="inlineStr">
@@ -1440,12 +1440,12 @@
       </c>
       <c r="C31" s="5" t="inlineStr">
         <is>
-          <t>Joint fluid analysis is a laboratory examination of fluid obtained from a joint.  The analysis assesses the fluid's appearance, cell count, and presence of crystals or microorganisms, helping to diagnose joint diseases.</t>
+          <t>It's a test that examines the fluid from a joint to check for problems.</t>
         </is>
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>Joint fluid analysis is performed when there is suspicion of joint inflammation, infection, or a specific type of arthritis.  It aids in differentiating between various causes of joint pain and swelling, guiding treatment decisions. The sample is usually obtained through arthrocentesis.</t>
+          <t>Doctors use this test when someone has joint pain, swelling, or other problems to find out what's causing them.</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr">
@@ -1475,12 +1475,12 @@
       </c>
       <c r="C32" s="6" t="inlineStr">
         <is>
-          <t>A kidney biopsy is a procedure where a small sample of kidney tissue is removed and examined under a microscope. This allows for the diagnosis and assessment of various kidney diseases and conditions affecting the structure and function of the kidneys.  The results help determine the severity and type of kidney damage.</t>
+          <t>It's a procedure where a small piece of kidney tissue is removed to be examined under a microscope.</t>
         </is>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>A kidney biopsy is performed when other tests suggest kidney disease, such as abnormal blood or urine tests, imaging findings, or symptoms like edema, hematuria, or proteinuria.  It helps determine the cause of kidney failure, monitor the effectiveness of treatment for kidney diseases, and evaluate the extent of kidney damage in various conditions. It is used to diagnose and stage glomerulonephritis, interstitial nephritis, and other kidney pathologies.</t>
+          <t>Doctors use this test when they suspect a problem with the kidneys, such as infection or disease.</t>
         </is>
       </c>
       <c r="E32" s="6" t="inlineStr">
@@ -1510,12 +1510,12 @@
       </c>
       <c r="C33" s="5" t="inlineStr">
         <is>
-          <t>Liver function tests (LFTs) are a group of blood tests that measure the levels of certain enzymes and proteins produced by the liver.  These tests assess liver health and detect potential liver damage or disease.</t>
+          <t>It's a blood test that checks how well your liver is working.</t>
         </is>
       </c>
       <c r="D33" s="5" t="inlineStr">
         <is>
-          <t>LFTs are ordered when there is a suspicion of liver disease, to monitor the progression of known liver conditions, or to assess the effects of medications on the liver. They help diagnose a wide range of conditions affecting the liver, from viral hepatitis and cirrhosis to alcohol-related liver disease and liver cancer.  The results can indicate the extent of liver damage and guide treatment decisions.</t>
+          <t>Doctors order it when they suspect a problem with your liver or to monitor liver health.</t>
         </is>
       </c>
       <c r="E33" s="5" t="inlineStr">
@@ -1545,12 +1545,12 @@
       </c>
       <c r="C34" s="6" t="inlineStr">
         <is>
-          <t>A lung diffusion test measures how well oxygen and carbon dioxide move between the lungs and the bloodstream. This assesses the efficiency of gas exchange in the lungs.</t>
+          <t>It's a test that checks how well your lungs take in oxygen.</t>
         </is>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use this test when they suspect problems with how your lungs work.</t>
         </is>
       </c>
       <c r="E34" s="6" t="inlineStr">
@@ -1580,12 +1580,12 @@
       </c>
       <c r="C35" s="5" t="inlineStr">
         <is>
-          <t>A lung volume test measures the amount of air your lungs can hold and how efficiently your lungs move air in and out.  It assesses lung function and helps diagnose various respiratory conditions.</t>
+          <t>It's a test that measures how much air your lungs can hold and how well they work.</t>
         </is>
       </c>
       <c r="D35" s="5" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use this test when they suspect a lung problem like asthma, or to check lung health before surgery.</t>
         </is>
       </c>
       <c r="E35" s="5" t="inlineStr">
@@ -1615,12 +1615,12 @@
       </c>
       <c r="C36" s="6" t="inlineStr">
         <is>
-          <t>Magnetic resonance angiography (MRA) is a non-invasive imaging technique that uses a magnetic field and radio waves to create detailed images of blood vessels.  It provides information about blood flow and the structure of arteries and veins, helping to identify blockages or abnormalities.</t>
+          <t>It's a scan that uses magnets and radio waves to take pictures of the blood vessels.</t>
         </is>
       </c>
       <c r="D36" s="6" t="inlineStr">
         <is>
-          <t>MRA is used to evaluate a wide range of vascular conditions. It is performed to diagnose or monitor diseases affecting blood vessels, such as aneurysms, stenosis, and vascular malformations.  The test helps clinicians assess blood flow, identify blockages, and guide treatment decisions. Information not found regarding specific conditions in this text.</t>
+          <t>Doctors use this scan to check for problems with blood flow in the arteries and veins.</t>
         </is>
       </c>
       <c r="E36" s="6" t="inlineStr">
@@ -1645,17 +1645,17 @@
       </c>
       <c r="B37" s="5" t="inlineStr">
         <is>
-          <t>Resonancia magnética nuclear; Imagen por resonancia magnética</t>
+          <t>Resonancia magnética</t>
         </is>
       </c>
       <c r="C37" s="5" t="inlineStr">
         <is>
-          <t>Magnetic resonance imaging (MRI) is a medical imaging technique that uses a powerful magnetic field and radio waves to create detailed images of the organs and structures within the body.  It provides cross-sectional views, allowing for visualization of soft tissues and internal structures with high resolution.</t>
+          <t>It's a scan that uses magnets and radio waves to take pictures of the inside of your body.</t>
         </is>
       </c>
       <c r="D37" s="5" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use it to see inside your body and check for problems in different organs and tissues.</t>
         </is>
       </c>
       <c r="E37" s="5" t="inlineStr">
@@ -1685,12 +1685,12 @@
       </c>
       <c r="C38" s="6" t="inlineStr">
         <is>
-          <t>Magnetic resonance venography (MRV) is a non-invasive imaging technique that uses magnetic fields and radio waves to create detailed images of the veins.  It assesses blood flow and identifies abnormalities within the veins, such as blood clots or stenosis.</t>
+          <t>It's a scan that uses magnets and radio waves to take pictures of the veins.</t>
         </is>
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
-          <t>MRV is used to diagnose and monitor venous conditions, particularly deep vein thrombosis (DVT), and to evaluate venous insufficiency. It is performed when there is suspicion of a blood clot, vein blockage, or other venous abnormalities based on patient symptoms or other diagnostic findings.  The test helps determine the extent of the venous problem, guiding treatment decisions.</t>
+          <t>Doctors use this scan to check for problems with blood flow in the veins.</t>
         </is>
       </c>
       <c r="E38" s="6" t="inlineStr">
@@ -1720,12 +1720,12 @@
       </c>
       <c r="C39" s="5" t="inlineStr">
         <is>
-          <t>A neurological evaluation is a comprehensive assessment of the nervous system. It involves a detailed history, neurological examination, and may include additional tests to identify neurological disorders or dysfunction. The goal is to pinpoint the location and nature of neurological problems.</t>
+          <t>It's a check-up of your brain and nerves to see how well they're working.</t>
         </is>
       </c>
       <c r="D39" s="5" t="inlineStr">
         <is>
-          <t>A neurological evaluation is performed when a patient presents with symptoms suggestive of neurological disease or injury. These symptoms can include weakness, numbness, tingling, difficulty with coordination, changes in vision or hearing, memory problems, seizures, or headaches.  The evaluation helps diagnose a wide range of conditions affecting the brain, spinal cord, nerves, and muscles.  It can guide treatment decisions and monitor disease progression.</t>
+          <t>Doctors use it when someone has problems with their brain, nerves, or muscles.</t>
         </is>
       </c>
       <c r="E39" s="5" t="inlineStr">
@@ -1755,12 +1755,12 @@
       </c>
       <c r="C40" s="6" t="inlineStr">
         <is>
-          <t>A neurological exam is a series of tests performed to assess the function of the nervous system.  It evaluates sensory, motor, and cognitive functions to identify potential neurological issues.  The exam may involve various assessments, including reflexes, coordination, and mental status.</t>
+          <t>It's a check-up of your nerves and brain to see how well they work.</t>
         </is>
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
-          <t>A neurological exam is used to detect, diagnose, and monitor a wide range of neurological conditions. It's performed when a patient presents with symptoms such as weakness, numbness, tingling, changes in vision or hearing, dizziness, difficulty with coordination, or cognitive impairment.  The exam helps determine the location and severity of neurological problems.  Information not found regarding specific conditions it helps *treat*.</t>
+          <t>Doctors use it to find problems with your brain, nerves, or muscles.</t>
         </is>
       </c>
       <c r="E40" s="6" t="inlineStr">
@@ -1785,17 +1785,17 @@
       </c>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t>Tomografía por emisión de positrones (TEP)</t>
+          <t>Gammagrafía por emisión de positrones</t>
         </is>
       </c>
       <c r="C41" s="5" t="inlineStr">
         <is>
-          <t>A PET scan is a nuclear medicine imaging technique that uses a radioactive tracer to visualize metabolic activity in the body.  It detects areas of increased metabolic activity, which can indicate the presence of disease.  The images produced are used to diagnose and monitor various medical conditions.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D41" s="5" t="inlineStr">
         <is>
-          <t>PET scans are used to detect and stage various cancers, assess the extent of disease spread, and monitor treatment response. They are also used to evaluate neurological disorders, cardiac conditions, and infections.  The procedure involves injecting a radioactive tracer that accumulates in areas of high metabolic activity, which are then detected by the scanner.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E41" s="5" t="inlineStr">
@@ -1825,12 +1825,12 @@
       </c>
       <c r="C42" s="6" t="inlineStr">
         <is>
-          <t>A physical exam is a non-invasive assessment of a patient's overall health.  It involves the physician visually inspecting, palpating, and auscultating various body systems to detect any abnormalities.  Findings from the physical exam guide further investigations or treatments.</t>
+          <t>A physical exam is when a doctor looks at your body and asks you questions to check your health.</t>
         </is>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>A physical exam is a fundamental part of any medical evaluation, used to screen for a wide range of conditions and assess a patient's general health status. It is performed to detect signs and symptoms of illness, monitor the progression of diseases, and evaluate the effectiveness of treatment.  It can help diagnose or assess many conditions depending on the findings.</t>
+          <t>Doctors use a physical exam to check for many health problems or to see how well you are doing.</t>
         </is>
       </c>
       <c r="E42" s="6" t="inlineStr">
@@ -1860,12 +1860,12 @@
       </c>
       <c r="C43" s="5" t="inlineStr">
         <is>
-          <t>A physical examination is a non-invasive procedure where a healthcare professional assesses a patient's overall health through visual inspection, palpation, auscultation, and percussion.  It involves evaluating various body systems to detect abnormalities or signs of disease.</t>
+          <t>A physical examination is when a doctor looks at and checks your body to see how healthy you are.</t>
         </is>
       </c>
       <c r="D43" s="5" t="inlineStr">
         <is>
-          <t>Physical examinations are a fundamental part of routine medical check-ups and are also performed to investigate specific symptoms or concerns. They are used to screen for diseases, monitor the progression of existing conditions, and guide further diagnostic testing.  The examination can reveal numerous potential health problems.</t>
+          <t>Doctors use a physical exam to check your overall health, find problems, or learn more about symptoms you have.</t>
         </is>
       </c>
       <c r="E43" s="5" t="inlineStr">
@@ -1895,12 +1895,12 @@
       </c>
       <c r="C44" s="6" t="inlineStr">
         <is>
-          <t>A pleural fluid culture is a laboratory test that involves growing microorganisms from a sample of pleural fluid.  This helps identify the presence and type of bacteria, fungi, or other infectious agents causing pleural infections.</t>
+          <t>It's a lab test that checks for germs in fluid around the lungs.</t>
         </is>
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>This test is performed when a patient presents with pleural effusion (fluid buildup in the pleural space) suspected to be infectious. It is crucial in determining the causative pathogen and guiding appropriate antibiotic therapy.  It aids in the diagnosis and management of various pleural infections, including pneumonia, empyema, and tuberculosis.</t>
+          <t>Doctors order this test when there's fluid around the lungs and they suspect an infection.</t>
         </is>
       </c>
       <c r="E44" s="6" t="inlineStr">
@@ -1930,12 +1930,12 @@
       </c>
       <c r="C45" s="5" t="inlineStr">
         <is>
-          <t>Pulse oximetry is a non-invasive method to measure the oxygen saturation of arterial blood.  It uses a sensor placed on a finger or toe to measure the percentage of hemoglobin saturated with oxygen. This simple test provides a quick assessment of oxygen levels in the body.</t>
+          <t>It's a simple test that measures how much oxygen is in your blood.</t>
         </is>
       </c>
       <c r="D45" s="5" t="inlineStr">
         <is>
-          <t>Pulse oximetry is used to monitor oxygen levels in various clinical settings, including during and after surgery, in patients with respiratory illnesses, and during exercise stress testing. It helps assess the effectiveness of oxygen therapy and identify conditions causing low blood oxygen (hypoxemia).  It is a crucial tool for monitoring patients at risk of respiratory compromise.</t>
+          <t>Doctors use this test to check how well your lungs and heart are working.</t>
         </is>
       </c>
       <c r="E45" s="5" t="inlineStr">
@@ -1960,17 +1960,17 @@
       </c>
       <c r="B46" s="6" t="inlineStr">
         <is>
-          <t>Prueba de marcha de seis minutos</t>
+          <t>Prueba de caminata de seis minutos</t>
         </is>
       </c>
       <c r="C46" s="6" t="inlineStr">
         <is>
-          <t>The six-minute walk test (6MWT) is a submaximal exercise test used to assess functional capacity and exercise tolerance.  It measures the distance a patient can walk in six minutes on a flat, hard surface.</t>
+          <t>It's a test where you walk as far as you can in six minutes to see how well your body works.</t>
         </is>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
-          <t>The 6MWT is used to evaluate the functional capacity of individuals with various cardiovascular and pulmonary conditions, as well as assessing disease progression and response to treatment. It's a simple, non-invasive test that can be performed in various settings, including clinics and hospitals.  It helps assess limitations in daily activities and overall fitness.</t>
+          <t>Doctors use this test to check how well your heart and lungs work, and to see how well you can exercise.</t>
         </is>
       </c>
       <c r="E46" s="6" t="inlineStr">
@@ -2000,12 +2000,12 @@
       </c>
       <c r="C47" s="5" t="inlineStr">
         <is>
-          <t>A spinal fluid examination is a diagnostic procedure that involves collecting and analyzing a sample of cerebrospinal fluid (CSF) from the spinal canal.  This analysis assesses the fluid's composition, helping identify various neurological conditions.</t>
+          <t>It's a test that checks the fluid surrounding the brain and spinal cord.</t>
         </is>
       </c>
       <c r="D47" s="5" t="inlineStr">
         <is>
-          <t>This test is used to diagnose and monitor conditions affecting the brain and spinal cord.  It is performed when symptoms suggest infection (meningitis, encephalitis), bleeding, multiple sclerosis, or other neurological disorders. The analysis evaluates cell counts, protein levels, glucose levels, and the presence of bacteria, viruses, or other abnormal substances.</t>
+          <t>Doctors order this test when they suspect a problem with the brain, spinal cord, or their coverings.</t>
         </is>
       </c>
       <c r="E47" s="5" t="inlineStr">
@@ -2035,12 +2035,12 @@
       </c>
       <c r="C48" s="6" t="inlineStr">
         <is>
-          <t>Spirometry is a pulmonary function test that measures the volume and flow of air during breathing.  It assesses lung capacity and airflow to diagnose and monitor respiratory conditions.</t>
+          <t>Spirometry is a breathing test that measures how well your lungs work.</t>
         </is>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
-          <t>Spirometry is used to evaluate respiratory symptoms such as shortness of breath, cough, and wheezing. It helps diagnose and monitor conditions affecting lung function, assess the severity of disease, and track response to treatment.  It is commonly used in the diagnosis and management of asthma, chronic obstructive pulmonary disease (COPD), and other pulmonary disorders.</t>
+          <t>Doctors use this test when they suspect you have lung problems like asthma or other breathing difficulties.</t>
         </is>
       </c>
       <c r="E48" s="6" t="inlineStr">
@@ -2065,17 +2065,17 @@
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>Examen de esputo; Análisis de esputo</t>
+          <t>Prueba de esputo</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
         <is>
-          <t>A sputum test is a laboratory examination of a sample of mucus coughed up from the respiratory tract.  It is used to identify the presence of microorganisms, cells, or other substances that may indicate a respiratory infection or other lung disease.  Microscopic examination and cultures are often performed on the sample.</t>
+          <t>A sputum test checks a sample of mucus from your lungs to look for germs or problems.</t>
         </is>
       </c>
       <c r="D49" s="5" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use this test when someone has a cough, lung problems, or to check for infections.</t>
         </is>
       </c>
       <c r="E49" s="5" t="inlineStr">
@@ -2105,12 +2105,12 @@
       </c>
       <c r="C50" s="6" t="inlineStr">
         <is>
-          <t>Thyroid function tests measure the levels of thyroid hormones (T3, T4, and TSH) in the blood.  These tests assess the thyroid gland's function, determining whether it's producing too much, too little, or the right amount of hormones. Results help diagnose and monitor thyroid disorders.</t>
+          <t>This blood test checks how well your thyroid gland is working.</t>
         </is>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
-          <t>These tests are ordered when symptoms suggest a thyroid problem, such as fatigue, weight changes, or changes in heart rate. They are used to diagnose hypothyroidism (underactive thyroid), hyperthyroidism (overactive thyroid), and other thyroid conditions.  They also monitor the effectiveness of thyroid hormone replacement therapy or other treatments.</t>
+          <t>Doctors order this test when they suspect a problem with your thyroid, like it's not making enough or too much hormone.</t>
         </is>
       </c>
       <c r="E50" s="6" t="inlineStr">
@@ -2135,17 +2135,17 @@
       </c>
       <c r="B51" s="5" t="inlineStr">
         <is>
-          <t>Ecografía; Ultrasonido</t>
+          <t>Ecografía</t>
         </is>
       </c>
       <c r="C51" s="5" t="inlineStr">
         <is>
-          <t>Ultrasound is a non-invasive diagnostic imaging technique that uses high-frequency sound waves to create images of internal organs and tissues.  It is used to visualize structures, assess blood flow, and detect abnormalities.</t>
+          <t>Ultrasound uses sound waves to create pictures of the inside of your body.</t>
         </is>
       </c>
       <c r="D51" s="5" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use ultrasound to look at organs and tissues to check for problems.</t>
         </is>
       </c>
       <c r="E51" s="5" t="inlineStr">
@@ -2170,17 +2170,17 @@
       </c>
       <c r="B52" s="6" t="inlineStr">
         <is>
-          <t>Análisis de orina; Examen de orina</t>
+          <t>Análisis de orina</t>
         </is>
       </c>
       <c r="C52" s="6" t="inlineStr">
         <is>
-          <t>A urine test is a laboratory analysis of a urine sample to detect abnormalities.  It assesses various components of urine, providing insights into overall health and potential underlying medical conditions.  Results can indicate the presence of infection, metabolic disorders, or kidney problems.</t>
+          <t>A urine test checks your urine for problems.</t>
         </is>
       </c>
       <c r="D52" s="6" t="inlineStr">
         <is>
-          <t>Urine tests are used to screen for and diagnose a wide range of conditions affecting the urinary tract, kidneys, and other systems. They are ordered when a patient presents with symptoms such as urinary tract infections, kidney stones, or changes in urination patterns.  It can help monitor the effectiveness of treatment for existing conditions.  It is also used for drug screening.</t>
+          <t>Doctors use this test to check for infections, kidney problems, or other health issues.</t>
         </is>
       </c>
       <c r="E52" s="6" t="inlineStr">
@@ -2205,17 +2205,17 @@
       </c>
       <c r="B53" s="5" t="inlineStr">
         <is>
-          <t>Análisis de orina; Exámenes de orina</t>
+          <t>Análisis de orina</t>
         </is>
       </c>
       <c r="C53" s="5" t="inlineStr">
         <is>
-          <t>Urine tests are laboratory analyses of a urine sample to detect various substances or abnormalities.  These tests assess kidney function, detect infections, and screen for metabolic disorders.  Results help diagnose and monitor a range of conditions.</t>
+          <t>Urine tests check your pee to find problems with your body.</t>
         </is>
       </c>
       <c r="D53" s="5" t="inlineStr">
         <is>
-          <t>Urine tests are ordered to evaluate kidney function, detect urinary tract infections (UTIs), screen for metabolic disorders (like diabetes), and monitor certain diseases. They're used to identify the presence of blood, protein, glucose, bacteria, and other substances not normally found in urine.  The results help diagnose or monitor conditions and guide treatment.</t>
+          <t>Doctors use urine tests to help find infections, kidney problems, or other health issues.</t>
         </is>
       </c>
       <c r="E53" s="5" t="inlineStr">
@@ -2240,17 +2240,17 @@
       </c>
       <c r="B54" s="6" t="inlineStr">
         <is>
-          <t>Medida de la circunferencia de la cintura;  Circunferencia abdominal</t>
+          <t>Medida de la circunferencia de la cintura</t>
         </is>
       </c>
       <c r="C54" s="6" t="inlineStr">
         <is>
-          <t>A waist circumference measurement is a simple anthropometric measurement of the circumference of the abdomen at the level of the umbilicus.  It is used as an indicator of abdominal adiposity and overall health risk.</t>
+          <t>It's measuring the size around your waist with a tape measure.</t>
         </is>
       </c>
       <c r="D54" s="6" t="inlineStr">
         <is>
-          <t>Waist circumference measurement is used to assess the amount of abdominal fat, which is a significant risk factor for several metabolic diseases. It is often performed as part of a routine physical examination or in the assessment of cardiovascular risk.  It helps screen for conditions related to excess abdominal fat.</t>
+          <t>Doctors use this measurement to check for extra fat around your belly, which can be a sign of health problems.</t>
         </is>
       </c>
       <c r="E54" s="6" t="inlineStr">
@@ -2280,12 +2280,12 @@
       </c>
       <c r="C55" s="5" t="inlineStr">
         <is>
-          <t>A radiograph, or X-ray, is a non-invasive medical imaging technique that uses ionizing radiation to produce images of internal body structures.  It reveals bone fractures, foreign bodies, and some soft tissue abnormalities.</t>
+          <t>An X-ray is a type of picture taken of the inside of your body using special rays.</t>
         </is>
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>X-rays are used to diagnose a wide range of conditions affecting bones, joints, lungs, and other tissues.  They are frequently performed to evaluate trauma, assess for infections, detect tumors, and monitor the progress of certain diseases.  The choice to perform an X-ray is based on the patient's symptoms, medical history, and the physician's clinical judgment.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr">
@@ -2432,12 +2432,12 @@
       </c>
       <c r="C9" s="11" t="inlineStr">
         <is>
-          <t>Acupuncture is a traditional Chinese medicine technique involving the insertion of thin needles into specific points on the body.  It aims to stimulate these points to alleviate pain, improve energy flow (Qi), and promote healing.  The purported mechanism involves the nervous and endocrine systems.</t>
+          <t>Acupuncture is a treatment where thin needles are put into the skin at specific points on the body.</t>
         </is>
       </c>
       <c r="D9" s="11" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use acupuncture to help relieve pain and other health problems.</t>
         </is>
       </c>
       <c r="E9" s="11" t="inlineStr">
@@ -2467,12 +2467,12 @@
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>Antibióticos are medications that combat bacterial infections by either killing bacteria or inhibiting their growth.  They are prescribed to treat a wide range of bacterial infections affecting various parts of the body.  The choice of antibiotic depends on the specific bacteria causing the infection and its susceptibility to various drugs.</t>
+          <t>Antibióticos son medicamentos que matan bacterias que causan infecciones.</t>
         </is>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
-          <t>Antibiotics are used to treat bacterial infections.  They are prescribed when a patient presents with symptoms suggestive of a bacterial infection, such as fever, inflammation, and localized or systemic signs of infection.  The choice of antibiotic is guided by factors such as the suspected pathogen, the patient's medical history, and antibiotic susceptibility testing (if available).  They are not effective against viral infections.</t>
+          <t>Los doctores recetan antibióticos cuando una persona tiene una infección bacteriana.</t>
         </is>
       </c>
       <c r="E10" s="6" t="inlineStr">
@@ -2497,17 +2497,17 @@
       </c>
       <c r="B11" s="11" t="inlineStr">
         <is>
-          <t>Información no encontrada (Information not found)</t>
+          <t>Información no encontrada</t>
         </is>
       </c>
       <c r="C11" s="11" t="inlineStr">
         <is>
-          <t>Information not found. The provided text describes a complete blood count (CBC), not assistive devices.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D11" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text describes a complete blood count (CBC), not assistive devices.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E11" s="11" t="inlineStr">
@@ -2537,12 +2537,12 @@
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>A behavior modification program is a type of psychotherapy that uses techniques to help individuals change undesirable behaviors.  It focuses on identifying triggers, developing coping mechanisms, and reinforcing positive behaviors.</t>
+          <t>It's a program that helps people learn new ways to behave.</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
-          <t>Behavior modification programs are used to treat a variety of behavioral and psychological disorders. They are employed when individuals exhibit maladaptive behaviors that negatively impact their lives and well-being. The goal is to replace negative behaviors with more adaptive ones through techniques such as positive reinforcement, shaping, and aversion therapy.</t>
+          <t>Doctors use it to help people with problems like anger, anxiety, or bad habits.</t>
         </is>
       </c>
       <c r="E12" s="6" t="inlineStr">
@@ -2572,12 +2572,12 @@
       </c>
       <c r="C13" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on complete blood counts and does not contain information about chondroitin.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D13" s="11" t="inlineStr">
         <is>
-          <t>Information not found.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E13" s="11" t="inlineStr">
@@ -2602,17 +2602,17 @@
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>Jarabe para la tos; Remedio para la tos</t>
+          <t>Remedio para la tos</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Cough medicine is a medication used to relieve cough symptoms.  It does not cure the underlying cause of the cough but aims to reduce its severity and frequency.  Different types of cough medicines target different cough mechanisms.</t>
+          <t>Cough medicine helps relieve coughing.</t>
         </is>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors give cough medicine when someone has a cough.</t>
         </is>
       </c>
       <c r="E14" s="6" t="inlineStr">
@@ -2642,12 +2642,12 @@
       </c>
       <c r="C15" s="11" t="inlineStr">
         <is>
-          <t>Dialysis is a procedure that removes waste products and excess fluid from the blood when the kidneys are unable to perform these functions adequately.  It's a life-sustaining treatment for individuals with end-stage renal disease.</t>
+          <t>Dialysis is a treatment that cleanses the blood when the kidneys don't work properly.</t>
         </is>
       </c>
       <c r="D15" s="11" t="inlineStr">
         <is>
-          <t>Dialysis is used when a person's kidneys are no longer functioning properly, leading to a buildup of toxins in the blood. It's performed to maintain a healthy balance of fluids and electrolytes in the body and prevent the accumulation of waste products that can cause serious health problems.  Dialysis can be a temporary measure or a long-term treatment depending on the underlying kidney condition.</t>
+          <t>Doctors use dialysis when a person's kidneys are failing and can't filter waste from their blood.</t>
         </is>
       </c>
       <c r="E15" s="11" t="inlineStr">
@@ -2677,12 +2677,12 @@
       </c>
       <c r="C16" s="6" t="inlineStr">
         <is>
-          <t>Dietary changes involve modifications to the types and amounts of food and beverages consumed.  This approach is used to improve health, manage existing conditions, or prevent future health issues.  It is often a cornerstone of treating various metabolic and nutritional disorders.</t>
+          <t>Dietary changes mean making different choices about the foods and drinks you eat.</t>
         </is>
       </c>
       <c r="D16" s="6" t="inlineStr">
         <is>
-          <t>Dietary changes are recommended for a wide range of health conditions, including obesity, diabetes, heart disease, and certain digestive disorders.  They are often prescribed to manage symptoms, improve overall health and wellness, and reduce the risk of chronic diseases. The specific changes are tailored to the individual's needs and health status.</t>
+          <t>Doctors suggest dietary changes to help people manage or prevent certain health problems.</t>
         </is>
       </c>
       <c r="E16" s="6" t="inlineStr">
@@ -2707,17 +2707,17 @@
       </c>
       <c r="B17" s="11" t="inlineStr">
         <is>
+          <t>Información no encontrada</t>
+        </is>
+      </c>
+      <c r="C17" s="11" t="inlineStr">
+        <is>
           <t>Information not found</t>
         </is>
       </c>
-      <c r="C17" s="11" t="inlineStr">
-        <is>
-          <t>Information not found. The provided text is about a complete blood count (CBC), not Donanemab-azbt.</t>
-        </is>
-      </c>
       <c r="D17" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text does not contain information about Donanemab-azbt.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E17" s="11" t="inlineStr">
@@ -2742,17 +2742,17 @@
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>Medicamento intravenoso de emergencia</t>
+          <t>Medicamentos intravenosos de emergencia</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>Emergency IV medicine refers to the administration of medications directly into a vein in a situation requiring immediate treatment.  This rapid delivery method ensures quick absorption and immediate therapeutic effects, vital in critical situations.</t>
+          <t>Emergency IV medicine is giving medicine directly into a vein through a needle.</t>
         </is>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t>Emergency IV medicine is used when a patient requires rapid treatment for life-threatening conditions or severe symptoms that necessitate immediate intervention.  It is employed to deliver medications that cannot be effectively absorbed through other routes, or when the speed of action is crucial.  The specific medications administered depend entirely on the patient's condition and the nature of the medical emergency.</t>
+          <t>Doctors use emergency IV medicine when someone is very sick and needs fast-acting treatment.</t>
         </is>
       </c>
       <c r="E18" s="6" t="inlineStr">
@@ -2777,17 +2777,17 @@
       </c>
       <c r="B19" s="11" t="inlineStr">
         <is>
-          <t>Participación en actividades placenteras</t>
+          <t>Realizar actividades placenteras</t>
         </is>
       </c>
       <c r="C19" s="11" t="inlineStr">
         <is>
-          <t>"Engaging in enjoyable activities" is not a medical test or procedure.  It is a behavioral intervention or recommendation sometimes used to improve mental and physical well-being.  It does not involve any physical examination or analysis.</t>
+          <t>This is not a medical test or procedure; it's a recommendation for improving well-being.</t>
         </is>
       </c>
       <c r="D19" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on a complete blood count (CBC) and does not contain information on the use of enjoyable activities as a medical intervention.</t>
+          <t>Doctors might suggest this to help manage stress, improve mood, and support overall health.</t>
         </is>
       </c>
       <c r="E19" s="11" t="inlineStr">
@@ -2817,12 +2817,12 @@
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on complete blood counts and does not contain information on "Environmental modifications" as a medical test or procedure.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D20" s="6" t="inlineStr">
         <is>
-          <t>Information not found.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E20" s="6" t="inlineStr">
@@ -2847,17 +2847,17 @@
       </c>
       <c r="B21" s="11" t="inlineStr">
         <is>
-          <t>Establecimiento de una rutina nocturna</t>
+          <t>Establecer una rutina nocturna</t>
         </is>
       </c>
       <c r="C21" s="11" t="inlineStr">
         <is>
-          <t>Establishing a nighttime routine is a behavioral intervention aimed at improving sleep hygiene and overall sleep quality.  It involves creating a consistent and relaxing set of pre-sleep activities to promote better sleep onset and maintenance.  This is not a medical test or procedure in the traditional sense.</t>
+          <t>It's a plan to help you sleep better at night.</t>
         </is>
       </c>
       <c r="D21" s="11" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors might suggest it if you have trouble sleeping or other sleep problems.</t>
         </is>
       </c>
       <c r="E21" s="11" t="inlineStr">
@@ -2882,17 +2882,17 @@
       </c>
       <c r="B22" s="6" t="inlineStr">
         <is>
-          <t>Información no encontrada (Information not found)</t>
+          <t>Información no encontrada</t>
         </is>
       </c>
       <c r="C22" s="6" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text describes a complete blood count (CBC), not exercise.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D22" s="6" t="inlineStr">
         <is>
-          <t>Information not found. The provided text describes a complete blood count (CBC), not exercise.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E22" s="6" t="inlineStr">
@@ -2917,17 +2917,17 @@
       </c>
       <c r="B23" s="11" t="inlineStr">
         <is>
-          <t>Antipiréticos/analgésicos</t>
+          <t>Reductores de fiebre/analgésicos</t>
         </is>
       </c>
       <c r="C23" s="11" t="inlineStr">
         <is>
-          <t>Fever reducers/pain relievers are medications used to reduce fever (antipyretic effect) and relieve pain (analgesic effect).  They are available over-the-counter and by prescription, with varying strengths and mechanisms of action.  They do not treat the underlying cause of fever or pain.</t>
+          <t>Fever reducers/pain relievers are medicines that help lower fever and reduce pain.</t>
         </is>
       </c>
       <c r="D23" s="11" t="inlineStr">
         <is>
-          <t>Fever reducers/pain relievers are used to manage symptoms of various illnesses and conditions causing fever and/or pain.  They are employed for symptomatic relief rather than curative treatment.  Use depends on the severity of symptoms and the individual's health status.  Conditions such as headaches, muscle aches, and flu often lead to their use.</t>
+          <t>Doctors give these medicines when someone has a fever or pain.</t>
         </is>
       </c>
       <c r="E23" s="11" t="inlineStr">
@@ -2957,12 +2957,12 @@
       </c>
       <c r="C24" s="6" t="inlineStr">
         <is>
-          <t>Fish oil is a dietary supplement derived from the tissues of oily fish.  It is a rich source of omega-3 fatty acids, EPA and DHA, which have various purported health benefits.  These benefits are not definitively proven through medical testing described in the provided text.</t>
+          <t>Fish oil is a type of supplement made from the oils of certain fish.</t>
         </is>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
-          <t>Information not found in provided text.  The provided text describes a complete blood count, not fish oil.</t>
+          <t>Doctors may recommend fish oil supplements to improve heart health or treat certain conditions.</t>
         </is>
       </c>
       <c r="E24" s="6" t="inlineStr">
@@ -2992,12 +2992,12 @@
       </c>
       <c r="C25" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text is about complete blood counts, not glucosamine.</t>
+          <t>Glucosamine is a supplement, not a medical test or procedure.</t>
         </is>
       </c>
       <c r="D25" s="11" t="inlineStr">
         <is>
-          <t>Information not found. The provided text is about complete blood counts, not glucosamine.</t>
+          <t>Doctors may recommend glucosamine supplements for joint pain.</t>
         </is>
       </c>
       <c r="E25" s="11" t="inlineStr">
@@ -3027,12 +3027,12 @@
       </c>
       <c r="C26" s="6" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on complete blood counts, not heart procedures.</t>
+          <t>Heart procedures are medical treatments done to fix problems with the heart.</t>
         </is>
       </c>
       <c r="D26" s="6" t="inlineStr">
         <is>
-          <t>Information not found. The provided text does not contain information on heart procedures.</t>
+          <t>Doctors use heart procedures when someone has a heart problem that needs fixing.</t>
         </is>
       </c>
       <c r="E26" s="6" t="inlineStr">
@@ -3062,12 +3062,12 @@
       </c>
       <c r="C27" s="11" t="inlineStr">
         <is>
-          <t>Heart surgery is a general term encompassing various surgical procedures performed on the heart and great vessels. These procedures aim to correct structural defects, repair damaged tissues, or alleviate conditions affecting cardiac function.</t>
+          <t>Heart surgery is an operation to fix problems with the heart.</t>
         </is>
       </c>
       <c r="D27" s="11" t="inlineStr">
         <is>
-          <t>Heart surgery is indicated for a wide range of cardiac conditions, including congenital heart defects, valvular heart disease, coronary artery disease (requiring coronary artery bypass grafting or CABG), and heart failure.  The specific type of surgery depends on the underlying diagnosis and the patient's overall health. It's performed to improve cardiac function, alleviate symptoms, and prolong life.</t>
+          <t>Doctors use heart surgery when the heart has a problem that medicine can't fix.</t>
         </is>
       </c>
       <c r="E27" s="11" t="inlineStr">
@@ -3092,17 +3092,17 @@
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>Terapia con calor y frío</t>
+          <t>Terapia de calor y frío</t>
         </is>
       </c>
       <c r="C28" s="6" t="inlineStr">
         <is>
-          <t>Heat and cold therapy involves the application of heat or cold to the body to treat various conditions.  Heat therapy promotes vasodilation and relaxation, while cold therapy reduces inflammation and numbs pain. This modality is used to manage pain and inflammation.</t>
+          <t>Heat and cold therapy uses heat or cold packs to ease pain and swelling.</t>
         </is>
       </c>
       <c r="D28" s="6" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use heat and cold therapy to help with pain and swelling from injuries or medical conditions.</t>
         </is>
       </c>
       <c r="E28" s="6" t="inlineStr">
@@ -3132,12 +3132,12 @@
       </c>
       <c r="C29" s="11" t="inlineStr">
         <is>
-          <t>A hospital stay refers to the period of time a patient spends in a hospital receiving medical care.  It encompasses a range of services, from diagnostic testing and treatment to surgery and recovery.  The length of a hospital stay varies greatly depending on the patient's condition and the required interventions.</t>
+          <t>A hospital stay is when someone spends time in a hospital for treatment or care.</t>
         </is>
       </c>
       <c r="D29" s="11" t="inlineStr">
         <is>
-          <t>Information not found in provided text.  The provided text describes a complete blood count, not a hospital stay.</t>
+          <t>Doctors use a hospital stay when someone needs close medical attention, such as after surgery or for a serious illness.</t>
         </is>
       </c>
       <c r="E29" s="11" t="inlineStr">
@@ -3167,12 +3167,12 @@
       </c>
       <c r="C30" s="6" t="inlineStr">
         <is>
-          <t>Hospitalization is the admission of a patient to a hospital for medical care, treatment, or observation.  It involves a stay of varying duration, depending on the patient's condition and the necessity for inpatient services.  Hospitalization provides access to a comprehensive range of medical resources and specialized care.</t>
+          <t>Hospitalization is a stay in a hospital for medical care.</t>
         </is>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>Information not found in provided text.</t>
+          <t>Doctors use hospitalization when someone needs close medical attention or treatment that can't be done at home.</t>
         </is>
       </c>
       <c r="E30" s="6" t="inlineStr">
@@ -3202,12 +3202,12 @@
       </c>
       <c r="C31" s="11" t="inlineStr">
         <is>
-          <t>Increased physical activity is not a medical test or procedure, but rather a lifestyle modification.  It involves engaging in more physical movement than usual, aiming to improve overall health and fitness.  This can range from moderate exercise to strenuous activities depending on individual goals and capabilities.</t>
+          <t>It's doing more physical activities like exercising or walking more.</t>
         </is>
       </c>
       <c r="D31" s="11" t="inlineStr">
         <is>
-          <t>Increased physical activity is recommended for the prevention and management of numerous health conditions. It is frequently prescribed as part of a comprehensive treatment plan to improve cardiovascular health, manage weight, and enhance mental well-being.  The specific type and intensity of activity are tailored to the individual's needs and health status.</t>
+          <t>Doctors might suggest this to help with some health problems or to improve your overall health.</t>
         </is>
       </c>
       <c r="E31" s="11" t="inlineStr">
@@ -3237,12 +3237,12 @@
       </c>
       <c r="C32" s="6" t="inlineStr">
         <is>
-          <t>A kidney transplant is a surgical procedure that involves replacing a diseased or damaged kidney with a healthy kidney from a donor.  This procedure is performed to restore kidney function and improve the overall health of individuals with end-stage renal disease.</t>
+          <t>A kidney transplant is a surgery where a healthy kidney is put into someone whose kidneys don't work well.</t>
         </is>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>Kidney transplantation is indicated for patients with end-stage renal disease (ESRD) who require renal replacement therapy.  It's performed to avoid the need for long-term dialysis and to improve the patient's quality of life. The procedure helps treat ESRD and its associated complications.  The choice of a living or deceased donor depends on several factors.</t>
+          <t>Doctors do a kidney transplant when someone's kidneys have failed and they need a new one to stay alive.</t>
         </is>
       </c>
       <c r="E32" s="6" t="inlineStr">
@@ -3272,12 +3272,12 @@
       </c>
       <c r="C33" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text discusses complete blood counts, not Lecanemab-irmb.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D33" s="11" t="inlineStr">
         <is>
-          <t>Information not found. The provided text focuses on complete blood counts and does not contain information about Lecanemab-irmb.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E33" s="11" t="inlineStr">
@@ -3307,12 +3307,12 @@
       </c>
       <c r="C34" s="6" t="inlineStr">
         <is>
-          <t>Lifestyle changes are non-invasive modifications to an individual's daily habits and behaviors.  These changes aim to improve overall health and reduce the risk of developing or worsening chronic diseases.  They encompass dietary adjustments, increased physical activity, stress management techniques, and smoking cessation.</t>
+          <t>Lifestyle changes are adjustments to how you live to improve your health.</t>
         </is>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>Lifestyle changes are recommended as a primary treatment or preventative measure for a wide array of health conditions. They are often employed to manage or prevent conditions such as obesity, hypertension, type 2 diabetes, cardiovascular disease, and certain cancers.  The specific changes recommended depend on the individual's health status, risk factors, and goals.  Lifestyle changes are a cornerstone of preventative medicine and are crucial for long-term health maintenance.</t>
+          <t>Doctors suggest lifestyle changes to help prevent or treat many health problems.</t>
         </is>
       </c>
       <c r="E34" s="6" t="inlineStr">
@@ -3337,17 +3337,17 @@
       </c>
       <c r="B35" s="11" t="inlineStr">
         <is>
-          <t>Manejo de complicaciones</t>
+          <t>Información no encontrada</t>
         </is>
       </c>
       <c r="C35" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text describes a complete blood count (CBC), a blood test, not "Managing complications."  "Managing complications" is a phrase referring to the treatment and care of problems arising from a disease or medical procedure, not a test or procedure itself.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D35" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on the CBC test.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E35" s="11" t="inlineStr">
@@ -3377,12 +3377,12 @@
       </c>
       <c r="C36" s="6" t="inlineStr">
         <is>
-          <t>Information not found in provided text.  Massage is a manual therapy technique involving the systematic manipulation of soft tissues.  Its purpose is to alleviate pain, improve circulation, and promote relaxation.</t>
+          <t>Massage is rubbing and kneading the body to relax muscles and ease pain.</t>
         </is>
       </c>
       <c r="D36" s="6" t="inlineStr">
         <is>
-          <t>Information not found in provided text. Massage therapy is used for a variety of purposes, including pain management, stress reduction, and improved range of motion.  It may be used as a complementary therapy alongside other medical treatments.</t>
+          <t>Doctors use massage to help people relax, reduce pain, and improve muscle function.</t>
         </is>
       </c>
       <c r="E36" s="6" t="inlineStr">
@@ -3482,12 +3482,12 @@
       </c>
       <c r="C39" s="11" t="inlineStr">
         <is>
-          <t>Occupational therapy is a type of therapy that helps people improve their ability to perform daily tasks.  It focuses on improving physical function, cognitive skills, and emotional well-being through engagement in purposeful activities.  The goal is to increase independence and quality of life.</t>
+          <t>Occupational therapy helps people improve their ability to do everyday tasks.</t>
         </is>
       </c>
       <c r="D39" s="11" t="inlineStr">
         <is>
-          <t>Occupational therapy is used to treat a wide range of conditions affecting physical, cognitive, or emotional function. It is used to help people recover from injuries, illnesses, or disabilities. The therapy is tailored to an individual's specific needs and goals, and may involve various techniques such as exercises, adaptive equipment, and environmental modifications.</t>
+          <t>Doctors use occupational therapy to help people recover from injuries, illnesses, or disabilities.</t>
         </is>
       </c>
       <c r="E39" s="11" t="inlineStr">
@@ -3517,12 +3517,12 @@
       </c>
       <c r="C40" s="6" t="inlineStr">
         <is>
-          <t>An outpatient treatment program provides medical care and therapeutic interventions to patients who do not require hospitalization.  It allows for regular monitoring and treatment while enabling the patient to maintain their normal daily life outside of a hospital setting.  These programs vary widely depending on the specific needs of the patient.</t>
+          <t>It's a program where you get medical care without needing to stay overnight in a hospital.</t>
         </is>
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on a complete blood count, not outpatient treatment programs.</t>
+          <t>Doctors use it when you need ongoing medical care but don't need to be in the hospital.</t>
         </is>
       </c>
       <c r="E40" s="6" t="inlineStr">
@@ -3552,12 +3552,12 @@
       </c>
       <c r="C41" s="11" t="inlineStr">
         <is>
-          <t>Oxygen therapy involves administering supplemental oxygen to increase the oxygen levels in a patient's blood. This is done to treat conditions causing low blood oxygen levels or to improve oxygen delivery to tissues.  It can be delivered via various methods including nasal cannula, mask, or ventilator.</t>
+          <t>Oxygen therapy is giving extra oxygen to help someone breathe better.</t>
         </is>
       </c>
       <c r="D41" s="11" t="inlineStr">
         <is>
-          <t>Oxygen therapy is used when a patient's blood oxygen saturation (SpO2) is low, indicating hypoxemia.  It is employed to treat a variety of respiratory and circulatory conditions that impair oxygen uptake and delivery.  It can be a short-term or long-term treatment depending on the underlying condition and its severity.</t>
+          <t>Doctors use oxygen therapy when someone has trouble getting enough oxygen from the air.</t>
         </is>
       </c>
       <c r="E41" s="11" t="inlineStr">
@@ -3587,12 +3587,12 @@
       </c>
       <c r="C42" s="6" t="inlineStr">
         <is>
-          <t>Physical therapy is a rehabilitative treatment that uses exercise, manual therapy, and other modalities to improve physical function, reduce pain, and restore mobility.  It aims to improve strength, flexibility, and range of motion in patients recovering from injury or managing chronic conditions.</t>
+          <t>Physical therapy helps people move better and feel less pain by doing exercises and other treatments.</t>
         </is>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors use physical therapy to help people recover from injuries, surgery, or illnesses that make it hard to move.</t>
         </is>
       </c>
       <c r="E42" s="6" t="inlineStr">
@@ -3622,12 +3622,12 @@
       </c>
       <c r="C43" s="11" t="inlineStr">
         <is>
-          <t>"Possibly surgery" is not a medical test or procedure itself, but rather an indication that surgical intervention might be necessary.  It represents a potential next step in a patient's care based on prior diagnostic testing and clinical evaluation.  The specifics of the surgery would depend entirely on the underlying medical condition.</t>
+          <t>It's a decision to see if an operation is needed.</t>
         </is>
       </c>
       <c r="D43" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The phrase "possibly surgery" does not provide enough information to describe background, usage, or conditions it helps with.  It's a conclusion or recommendation following other diagnostic assessments, not a test or procedure in itself.</t>
+          <t>Doctors may suggest surgery if other treatments haven't worked or if a serious problem needs fixing.</t>
         </is>
       </c>
       <c r="E43" s="11" t="inlineStr">
@@ -3657,12 +3657,12 @@
       </c>
       <c r="C44" s="6" t="inlineStr">
         <is>
-          <t>Psicoterapia is a talking therapy involving a trained professional to help individuals understand and manage their mental health conditions.  It uses various techniques to address emotional, behavioral, and cognitive issues, promoting improved mental well-being.</t>
+          <t>Psychotherapy is a type of talking therapy that helps people cope with mental health issues.</t>
         </is>
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>Psychotherapy is used to treat a wide range of mental health disorders and emotional difficulties. It is performed to address symptoms such as anxiety, depression, trauma, relationship problems, and substance abuse.  The specific approach used depends on the individual's needs and the therapist's expertise.</t>
+          <t>Doctors use psychotherapy to help people with emotional problems, relationship difficulties, or mental illnesses.</t>
         </is>
       </c>
       <c r="E44" s="6" t="inlineStr">
@@ -3692,12 +3692,12 @@
       </c>
       <c r="C45" s="11" t="inlineStr">
         <is>
-          <t>Quitting smoking is a behavioral intervention aimed at cessation of tobacco use. It involves strategies to manage withdrawal symptoms and cravings, ultimately reducing or eliminating nicotine dependence.  This process can significantly improve various health outcomes.</t>
+          <t>Quitting smoking is stopping the habit of smoking cigarettes or other tobacco products.</t>
         </is>
       </c>
       <c r="D45" s="11" t="inlineStr">
         <is>
-          <t>Quitting smoking is recommended for individuals with a history of smoking, especially those experiencing smoking-related health problems or seeking to prevent future health issues.  It is performed to reduce the risk of developing or worsening numerous diseases caused by tobacco use. This intervention helps treat and prevent a wide array of conditions linked to smoking.</t>
+          <t>Doctors suggest quitting smoking to improve a person's health and reduce the risk of many diseases.</t>
         </is>
       </c>
       <c r="E45" s="11" t="inlineStr">
@@ -3727,12 +3727,12 @@
       </c>
       <c r="C46" s="6" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text describes a complete blood count (CBC), not "Simpler tasks and structured routines."  The phrase "Simpler tasks and structured routines" does not refer to a medical test or procedure.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
-          <t>Information not found.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E46" s="6" t="inlineStr">
@@ -3757,17 +3757,17 @@
       </c>
       <c r="B47" s="11" t="inlineStr">
         <is>
-          <t>Terapia del habla; Logopedia</t>
+          <t>Terapia del habla</t>
         </is>
       </c>
       <c r="C47" s="11" t="inlineStr">
         <is>
-          <t>Speech therapy is a therapeutic intervention aimed at improving communication and swallowing disorders.  It involves exercises and strategies to enhance articulation, fluency, voice, and language skills.  It may also address swallowing difficulties (dysphagia).</t>
+          <t>Speech therapy helps people improve how they speak, understand, and communicate.</t>
         </is>
       </c>
       <c r="D47" s="11" t="inlineStr">
         <is>
-          <t>Speech therapy is utilized when individuals experience difficulties with speech production, language comprehension or expression, fluency, voice quality, or swallowing.  It's performed to improve communication abilities, enhance quality of life, and address underlying medical conditions affecting speech and swallowing. This therapy can help diagnose and treat a wide range of communication and swallowing disorders across the lifespan.</t>
+          <t>Doctors use speech therapy when someone has trouble speaking, understanding, or communicating because of a medical condition or injury.</t>
         </is>
       </c>
       <c r="E47" s="11" t="inlineStr">
@@ -3792,17 +3792,17 @@
       </c>
       <c r="B48" s="6" t="inlineStr">
         <is>
-          <t>Cirugía</t>
+          <t>Información no encontrada</t>
         </is>
       </c>
       <c r="C48" s="6" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text describes a complete blood count (CBC), not surgery.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
-          <t>Information not found. The provided text describes a complete blood count (CBC), not surgery.</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="E48" s="6" t="inlineStr">
@@ -3827,17 +3827,17 @@
       </c>
       <c r="B49" s="11" t="inlineStr">
         <is>
-          <t>Tai chi (The Spanish translation is the same as the English term)</t>
+          <t>Tai chi (This term doesn't require translation as it's already used in Spanish)</t>
         </is>
       </c>
       <c r="C49" s="11" t="inlineStr">
         <is>
-          <t>Tai chi is a mind-body practice that involves a series of slow, gentle movements and deep breathing exercises. It is used to improve physical health, balance, and mental well-being.</t>
+          <t>Tai chi is a type of gentle exercise that involves slow, flowing movements.</t>
         </is>
       </c>
       <c r="D49" s="11" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors may recommend tai chi to help improve balance, flexibility, and reduce stress.</t>
         </is>
       </c>
       <c r="E49" s="11" t="inlineStr">
@@ -3867,12 +3867,12 @@
       </c>
       <c r="C50" s="6" t="inlineStr">
         <is>
-          <t>"Treating the underlying cause" is not a medical test or procedure itself, but rather a therapeutic goal.  It refers to identifying and addressing the root cause of a medical condition, rather than just treating the symptoms. This approach is crucial for effective and long-term health management.</t>
+          <t>This isn't a test or procedure; it's a goal of medical treatment — fixing the problem causing the illness.</t>
         </is>
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
-          <t>This approach is used when a patient presents with symptoms indicating an underlying medical issue.  The goal is to identify the root cause through various diagnostic tests and investigations (such as the complete blood count mentioned in the provided text) to determine the appropriate treatment strategy.  This may involve medication, surgery, lifestyle changes, or a combination of these. It helps in preventing recurrence of the symptoms and improving overall health outcomes.</t>
+          <t>Doctors aim to treat the underlying cause when someone is sick to make them better.</t>
         </is>
       </c>
       <c r="E50" s="6" t="inlineStr">
@@ -3902,12 +3902,12 @@
       </c>
       <c r="C51" s="11" t="inlineStr">
         <is>
-          <t>Weight loss is a reduction in body mass, often expressed as a decrease in body weight.  It can be intentional, such as through dieting or exercise, or unintentional, indicating an underlying medical condition.  The process itself is not a test or procedure, but rather a potential symptom or outcome.</t>
+          <t>Weight loss is when someone gets lighter because they are eating less or exercising more.</t>
         </is>
       </c>
       <c r="D51" s="11" t="inlineStr">
         <is>
-          <t>Information not found.  The provided text focuses on complete blood counts, not weight loss.</t>
+          <t>Doctors might suggest weight loss to help people with health problems like high blood pressure or diabetes.</t>
         </is>
       </c>
       <c r="E51" s="11" t="inlineStr">
@@ -3937,12 +3937,12 @@
       </c>
       <c r="C52" s="6" t="inlineStr">
         <is>
-          <t>Yoga is a mind-body practice that combines physical postures, breathing techniques, and meditation.  It aims to improve physical flexibility, strength, and balance, while also promoting mental well-being and stress reduction.  It is not a medical test or procedure.</t>
+          <t>Yoga is a type of exercise that involves poses and breathing.</t>
         </is>
       </c>
       <c r="D52" s="6" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Doctors may recommend yoga to help with stress, flexibility, and some health problems.</t>
         </is>
       </c>
       <c r="E52" s="6" t="inlineStr">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>47 / 47 (100.0%)</t>
+          <t>46 / 47 (97.9%)</t>
         </is>
       </c>
     </row>

</xml_diff>